<commit_message>
Añadiendo unos nuevos destinos
Destinos nuevos a tres tabs de Excel
</commit_message>
<xml_diff>
--- a/Primer Desafio Practico/Ejercicio 1/Los Top 100.xlsx
+++ b/Primer Desafio Practico/Ejercicio 1/Los Top 100.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\DOCUMENTOS CUQUIS\UNIVERSIDAD\CICLO 04\Dataware Y Mineria de datos\Laboratorio-de-Datawarehouse\Primer Desafio Practico\Ejercicio 1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{3C24520E-4BF4-4B58-B0C1-F502E9A84618}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2CCC824D-2CE0-4FD3-A162-08167C78B731}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{2F5FEEE0-2581-4495-A908-044A7BEE2A44}"/>
+    <workbookView xWindow="2160" yWindow="2160" windowWidth="15375" windowHeight="7980" xr2:uid="{2F5FEEE0-2581-4495-A908-044A7BEE2A44}"/>
   </bookViews>
   <sheets>
-    <sheet name="Top 100" sheetId="1" r:id="rId1"/>
-    <sheet name="Top 100 Hombres" sheetId="2" r:id="rId2"/>
-    <sheet name="Top 100 Mujeres" sheetId="3" r:id="rId3"/>
+    <sheet name="Orden por ingresos" sheetId="1" r:id="rId1"/>
+    <sheet name="Orden por Ingreso siendo hombre" sheetId="2" r:id="rId2"/>
+    <sheet name="Orden por ingreso siendo mujer" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -407,7 +407,7 @@
   <dimension ref="A1:B1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -466,7 +466,7 @@
   <dimension ref="A1:F1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>